<commit_message>
chore: added new intersection tables, removed files saved in wrong places
</commit_message>
<xml_diff>
--- a/results/tables/number_of_samples.xlsx
+++ b/results/tables/number_of_samples.xlsx
@@ -32,25 +32,25 @@
     <t xml:space="preserve">female</t>
   </si>
   <si>
+    <t xml:space="preserve">Cg25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MDD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OFC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sub</t>
+  </si>
+  <si>
     <t xml:space="preserve">aINS</t>
   </si>
   <si>
-    <t xml:space="preserve">MDD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cg25</t>
-  </si>
-  <si>
     <t xml:space="preserve">dlPFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nac</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OFC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sub</t>
   </si>
   <si>
     <t xml:space="preserve">male</t>
@@ -410,7 +410,7 @@
         <v>6</v>
       </c>
       <c r="D2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3">
@@ -424,7 +424,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
@@ -438,7 +438,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -452,7 +452,7 @@
         <v>8</v>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6">
@@ -480,7 +480,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -494,7 +494,7 @@
         <v>10</v>
       </c>
       <c r="D8" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
@@ -508,7 +508,7 @@
         <v>10</v>
       </c>
       <c r="D9" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
@@ -536,7 +536,7 @@
         <v>11</v>
       </c>
       <c r="D11" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12">
@@ -550,7 +550,7 @@
         <v>12</v>
       </c>
       <c r="D12" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
@@ -564,7 +564,7 @@
         <v>12</v>
       </c>
       <c r="D13" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
@@ -578,7 +578,7 @@
         <v>6</v>
       </c>
       <c r="D14" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15">
@@ -592,7 +592,7 @@
         <v>6</v>
       </c>
       <c r="D15" t="n">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
@@ -606,7 +606,7 @@
         <v>8</v>
       </c>
       <c r="D16" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
@@ -620,7 +620,7 @@
         <v>8</v>
       </c>
       <c r="D17" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18">
@@ -662,7 +662,7 @@
         <v>10</v>
       </c>
       <c r="D20" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21">
@@ -676,7 +676,7 @@
         <v>10</v>
       </c>
       <c r="D21" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22">
@@ -704,7 +704,7 @@
         <v>11</v>
       </c>
       <c r="D23" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24">
@@ -718,7 +718,7 @@
         <v>12</v>
       </c>
       <c r="D24" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25">
@@ -732,7 +732,7 @@
         <v>12</v>
       </c>
       <c r="D25" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>